<commit_message>
desafio 14 corregido sin probar
</commit_message>
<xml_diff>
--- a/desafio.clase.14/Funcionalidades y controles.xlsx
+++ b/desafio.clase.14/Funcionalidades y controles.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\desafio.clase.14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6D2E8FB-E32A-4133-801D-5DA9306936BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AECCBB-3BEC-4DCE-8506-5CE1F9EB0C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F0CF4C01-9251-45F7-B63D-D19EBD064942}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{F0CF4C01-9251-45F7-B63D-D19EBD064942}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="productos" sheetId="1" r:id="rId1"/>
+    <sheet name="carritos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>GET /api/productos</t>
   </si>
@@ -76,9 +77,6 @@
     <t>1) se le pasa un objeto, y debe retornar el objeto actualizado</t>
   </si>
   <si>
-    <t>3) el timestamp se debe actualizar al retornar el objeto actualizado</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -101,6 +99,72 @@
   </si>
   <si>
     <t>2) solo debe aceptar las propiedades de un producto (el crud solo debe tomar las caracteristicas necesarias)</t>
+  </si>
+  <si>
+    <t>POST api/carrito</t>
+  </si>
+  <si>
+    <t>1) crea carrito y devuelve id</t>
+  </si>
+  <si>
+    <t>2) si el archivo no existe, debe dar error</t>
+  </si>
+  <si>
+    <t>DELETE api/carrito/:id</t>
+  </si>
+  <si>
+    <t>1) vacia un carrito y lo elimina</t>
+  </si>
+  <si>
+    <t>2) si el carrito no existe, debe dar error</t>
+  </si>
+  <si>
+    <t>3) si el archivo no existe, debe dar error</t>
+  </si>
+  <si>
+    <t>GET api/carrito/:id/productos</t>
+  </si>
+  <si>
+    <t>1) debe devolver los productos del carrito</t>
+  </si>
+  <si>
+    <t>3) si el carrito no existe, debe dar mensaje de error</t>
+  </si>
+  <si>
+    <t>4) si el archivo no existe, debe dar error</t>
+  </si>
+  <si>
+    <t>POST api/carrito/:id/productos</t>
+  </si>
+  <si>
+    <t>1) tiene que incorporar productos al carrito por su id, devuelve el carrito con los productos</t>
+  </si>
+  <si>
+    <t>2) si el producto no existe, debe devolver error</t>
+  </si>
+  <si>
+    <t>3) si el carrito no existe, debe devolver error</t>
+  </si>
+  <si>
+    <t>4) si alguno de los 2 archivos no existe, debe dar error</t>
+  </si>
+  <si>
+    <t>1) debe eliminar producto del carrito con ambos id, devuelve el carrito sin el producto</t>
+  </si>
+  <si>
+    <t>3) si el producto no existe en el carrito, debe dar error</t>
+  </si>
+  <si>
+    <t>4) si el archivo de carrito no existe, debe dar error</t>
+  </si>
+  <si>
+    <t>2) si el carrito esta vacio, devuelve un error de carrito vacio</t>
+  </si>
+  <si>
+    <t>DELETE api/carrito/:id/productos/:idprod</t>
+  </si>
+  <si>
+    <t>3) el timestamp se debe actualizar al retornar el objeto actualizado (???)</t>
   </si>
 </sst>
 </file>
@@ -461,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53E6B018-E5B1-4D7A-8C2F-FFEB1A33BCCA}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,7 +556,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -610,7 +674,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -630,12 +694,12 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -650,7 +714,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -665,17 +729,17 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -690,7 +754,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -706,4 +770,265 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD88EDC2-22C2-4D6E-A70F-9549391C3ADF}">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>